<commit_message>
gpu convolution under development
</commit_message>
<xml_diff>
--- a/3D-GreenIterations/results/error-tables.xlsx
+++ b/3D-GreenIterations/results/error-tables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14740" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14740" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GreenIteration" sheetId="1" r:id="rId1"/>
     <sheet name="EnergyComputation" sheetId="2" r:id="rId2"/>
+    <sheet name="cudaPython" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="44">
   <si>
     <t>numpts / boxsize</t>
   </si>
@@ -142,17 +143,34 @@
   </si>
   <si>
     <t>These results are converging, but the number of cell is unreasonably high when the variation tolerance is that low.  Example, 126288 after the 5th refinement, and many cells would like to be funrther refined if allowed.</t>
+  </si>
+  <si>
+    <t>Compute N^2 interactions for N randomly distributed targets and N randomly distributed sources in [0,1]x[0,1]x[0,1]</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>speedup</t>
+  </si>
+  <si>
+    <t>cpu  time (s)</t>
+  </si>
+  <si>
+    <t>gpu time (s)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.000000"/>
-    <numFmt numFmtId="170" formatCode="0.0000000"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -189,6 +207,35 @@
       <color theme="1"/>
       <name val="Monaco"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -233,12 +280,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -249,22 +293,67 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -704,10 +793,10 @@
       </c>
     </row>
     <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="2"/>
       <c r="D3" s="1">
         <v>4</v>
@@ -760,8 +849,8 @@
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="2"/>
       <c r="D4" s="1">
         <v>6</v>
@@ -814,8 +903,8 @@
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="2"/>
       <c r="D5" s="1">
         <v>8</v>
@@ -868,8 +957,8 @@
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="2"/>
       <c r="D6" s="1">
         <v>10</v>
@@ -922,8 +1011,8 @@
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="2"/>
       <c r="D7" s="1">
         <v>12</v>
@@ -976,8 +1065,8 @@
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="2"/>
       <c r="D8" s="1">
         <v>14</v>
@@ -1030,8 +1119,8 @@
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="2"/>
       <c r="D9" s="1">
         <v>16</v>
@@ -1084,8 +1173,8 @@
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="2"/>
       <c r="D10" s="1">
         <v>18</v>
@@ -1108,24 +1197,24 @@
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="2"/>
       <c r="D11" s="1">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="2"/>
       <c r="D12" s="1">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="2"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
@@ -1358,633 +1447,633 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D30FA40-3F0B-5D4C-8BF8-3F0335D8AB3A}">
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="4"/>
-    <col min="2" max="2" width="19.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="4"/>
-    <col min="5" max="5" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="19.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="3"/>
+    <col min="5" max="5" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>6</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="8">
         <v>2.4077908905000001E-2</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="8">
         <v>2.3570959345899999E-2</v>
       </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>8</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="8">
         <v>2.4005161336699998E-2</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="8">
         <v>2.3500627115700001E-2</v>
       </c>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>10</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="8">
         <v>2.40034119985E-2</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="8">
         <v>2.3498939373299998E-2</v>
       </c>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>12</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="8">
         <v>2.4003372371999999E-2</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G15" s="8">
         <v>2.3498901189399998E-2</v>
       </c>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="7" t="s">
+      <c r="I19" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="3">
         <v>6</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="7">
         <v>2.0962814330500001E-3</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="7">
         <v>1.0018950388500001E-3</v>
       </c>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="3">
         <v>8</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="7">
         <v>1.9992784341400002E-3</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="7">
         <v>9.0582004173599996E-4</v>
       </c>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="3">
         <v>10</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22" s="7">
         <v>1.99691323748E-3</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="7">
         <v>9.0347870030800005E-4</v>
       </c>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
     </row>
     <row r="26" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="G26" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="27" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="3">
         <v>6</v>
       </c>
-      <c r="F27" s="10">
+      <c r="F27" s="8">
         <v>3.8774649088500002E-3</v>
       </c>
-      <c r="G27" s="10">
+      <c r="G27" s="8">
         <v>5.03297188896E-3</v>
       </c>
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="3">
         <v>8</v>
       </c>
-      <c r="F28" s="10">
+      <c r="F28" s="8">
         <v>3.76726657446E-3</v>
       </c>
-      <c r="G28" s="10">
+      <c r="G28" s="8">
         <v>5.41325877415E-3</v>
       </c>
     </row>
     <row r="29" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
     </row>
     <row r="30" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E34" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="F34" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G34" s="8" t="s">
+      <c r="G34" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E35" s="4">
+      <c r="E35" s="3">
         <v>0.2</v>
       </c>
-      <c r="F35" s="11">
+      <c r="F35" s="9">
         <v>2.0245116348200001E-2</v>
       </c>
-      <c r="G35" s="11">
+      <c r="G35" s="9">
         <v>2.4287744138799999E-2</v>
       </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E36" s="3">
         <v>0.15</v>
       </c>
-      <c r="F36" s="11">
+      <c r="F36" s="9">
         <v>9.7475152777400001E-4</v>
       </c>
-      <c r="G36" s="11">
+      <c r="G36" s="9">
         <v>4.7406991060899998E-3</v>
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E37" s="3">
         <v>0.1</v>
       </c>
-      <c r="F37" s="11">
+      <c r="F37" s="9">
         <v>1.9992784341400002E-3</v>
       </c>
-      <c r="G37" s="11">
+      <c r="G37" s="9">
         <v>9.0582004173599996E-4</v>
       </c>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E38" s="4">
+      <c r="E38" s="3">
         <v>0.05</v>
       </c>
-      <c r="F38" s="6">
+      <c r="F38" s="5">
         <v>5.4313821231099998E-3</v>
       </c>
-      <c r="G38" s="6">
+      <c r="G38" s="5">
         <v>4.9913416201399999E-3</v>
       </c>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C42" s="8" t="s">
+      <c r="C42" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="E42" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F42" s="8" t="s">
+      <c r="F42" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G42" s="8" t="s">
+      <c r="G42" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E43" s="4">
+      <c r="E43" s="3">
         <v>0.5</v>
       </c>
-      <c r="F43" s="11" t="s">
+      <c r="F43" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G43" s="6">
+      <c r="G43" s="5">
         <v>0.21473642317700001</v>
       </c>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E44" s="4">
+      <c r="E44" s="3">
         <v>0.1</v>
       </c>
-      <c r="F44" s="11" t="s">
+      <c r="F44" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G44" s="6">
+      <c r="G44" s="5">
         <v>2.7015191971599999E-2</v>
       </c>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E45" s="4">
+      <c r="E45" s="3">
         <v>0.05</v>
       </c>
-      <c r="F45" s="11" t="s">
+      <c r="F45" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G45" s="6">
+      <c r="G45" s="5">
         <v>8.3256710788400003E-3</v>
       </c>
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E46" s="4">
+      <c r="E46" s="3">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F46" s="11" t="s">
+      <c r="F46" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G46" s="6">
+      <c r="G46" s="5">
         <v>1.7500669738900001E-3</v>
       </c>
     </row>
     <row r="50" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C50" s="8" t="s">
+      <c r="C50" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E50" s="8" t="s">
+      <c r="E50" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F50" s="8" t="s">
+      <c r="F50" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G50" s="8" t="s">
+      <c r="G50" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="51" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E51" s="4">
+      <c r="E51" s="3">
         <v>0.5</v>
       </c>
-      <c r="F51" s="11" t="s">
+      <c r="F51" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G51" s="6">
+      <c r="G51" s="5">
         <v>0.222468738897</v>
       </c>
     </row>
     <row r="52" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E52" s="4">
+      <c r="E52" s="3">
         <v>0.1</v>
       </c>
-      <c r="F52" s="11" t="s">
+      <c r="F52" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G52" s="6">
+      <c r="G52" s="5">
         <v>3.8126772905099998E-2</v>
       </c>
     </row>
     <row r="53" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E53" s="4">
+      <c r="E53" s="3">
         <v>0.05</v>
       </c>
-      <c r="F53" s="11" t="s">
+      <c r="F53" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G53" s="6">
+      <c r="G53" s="5">
         <v>1.9759926649899999E-2</v>
       </c>
     </row>
     <row r="54" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E54" s="4">
+      <c r="E54" s="3">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F54" s="11" t="s">
+      <c r="F54" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G54" s="6">
+      <c r="G54" s="5">
         <v>1.2812395644700001E-2</v>
       </c>
     </row>
     <row r="58" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C58" s="8" t="s">
+      <c r="C58" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E58" s="8" t="s">
+      <c r="E58" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F58" s="8" t="s">
+      <c r="F58" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G58" s="8" t="s">
+      <c r="G58" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="59" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C59" s="4" t="s">
+      <c r="C59" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E59" s="4">
+      <c r="E59" s="3">
         <v>0.2</v>
       </c>
-      <c r="F59" s="6">
+      <c r="F59" s="5">
         <v>3.1553131115700003E-2</v>
       </c>
-      <c r="G59" s="6">
+      <c r="G59" s="5">
         <v>1.4138246648400001E-2</v>
       </c>
-      <c r="I59" s="7" t="s">
+      <c r="I59" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="J59" s="7"/>
-      <c r="K59" s="7"/>
-      <c r="L59" s="7"/>
+      <c r="J59" s="13"/>
+      <c r="K59" s="13"/>
+      <c r="L59" s="13"/>
     </row>
     <row r="60" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C60" s="4" t="s">
+      <c r="C60" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E60" s="4">
+      <c r="E60" s="3">
         <v>0.15</v>
       </c>
-      <c r="F60" s="6">
+      <c r="F60" s="5">
         <v>1.34187266104E-2</v>
       </c>
-      <c r="G60" s="6">
+      <c r="G60" s="5">
         <v>1.7598548207299999E-2</v>
       </c>
-      <c r="I60" s="7"/>
-      <c r="J60" s="7"/>
-      <c r="K60" s="7"/>
-      <c r="L60" s="7"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="13"/>
+      <c r="K60" s="13"/>
+      <c r="L60" s="13"/>
     </row>
     <row r="61" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C61" s="4" t="s">
+      <c r="C61" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E61" s="4">
+      <c r="E61" s="3">
         <v>0.1</v>
       </c>
-      <c r="F61" s="6">
+      <c r="F61" s="5">
         <v>4.9455563717099998E-3</v>
       </c>
-      <c r="G61" s="6">
+      <c r="G61" s="5">
         <v>1.2812395644700001E-2</v>
       </c>
-      <c r="I61" s="7"/>
-      <c r="J61" s="7"/>
-      <c r="K61" s="7"/>
-      <c r="L61" s="7"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="13"/>
+      <c r="K61" s="13"/>
+      <c r="L61" s="13"/>
     </row>
     <row r="62" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C62" s="4" t="s">
+      <c r="C62" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E62" s="4">
+      <c r="E62" s="3">
         <v>0.05</v>
       </c>
-      <c r="F62" s="6">
+      <c r="F62" s="5">
         <v>1.30416231706E-3</v>
       </c>
-      <c r="G62" s="6">
+      <c r="G62" s="5">
         <v>6.7289220777000001E-3</v>
       </c>
-      <c r="I62" s="7"/>
-      <c r="J62" s="7"/>
-      <c r="K62" s="7"/>
-      <c r="L62" s="7"/>
+      <c r="I62" s="13"/>
+      <c r="J62" s="13"/>
+      <c r="K62" s="13"/>
+      <c r="L62" s="13"/>
     </row>
     <row r="63" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="E63" s="4">
+      <c r="E63" s="3">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F63" s="12">
+      <c r="F63" s="10">
         <v>4.3491369457099999E-5</v>
       </c>
-      <c r="G63" s="6">
+      <c r="G63" s="5">
         <v>4.3757631963099999E-3</v>
       </c>
-      <c r="I63" s="7"/>
-      <c r="J63" s="7"/>
-      <c r="K63" s="7"/>
-      <c r="L63" s="7"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="13"/>
+      <c r="K63" s="13"/>
+      <c r="L63" s="13"/>
     </row>
     <row r="64" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="I64" s="7"/>
-      <c r="J64" s="7"/>
-      <c r="K64" s="7"/>
-      <c r="L64" s="7"/>
+      <c r="I64" s="13"/>
+      <c r="J64" s="13"/>
+      <c r="K64" s="13"/>
+      <c r="L64" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2188,4 +2277,384 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B080905A-CA13-964F-A94E-4C77543CC85C}">
+  <dimension ref="A1:G31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="4"/>
+    <col min="2" max="2" width="10.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" style="4" customWidth="1"/>
+    <col min="7" max="7" width="34" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="25"/>
+    </row>
+    <row r="2" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="25"/>
+    </row>
+    <row r="3" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="25"/>
+    </row>
+    <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+    </row>
+    <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B6" s="16">
+        <v>128</v>
+      </c>
+      <c r="C6" s="17">
+        <v>4.9127999999999998E-2</v>
+      </c>
+      <c r="D6" s="17">
+        <v>0.57667500000000005</v>
+      </c>
+      <c r="E6" s="18">
+        <f t="shared" ref="E6:E7" si="0">C6/D6</f>
+        <v>8.5191832487969812E-2</v>
+      </c>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+    </row>
+    <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B7" s="16">
+        <v>256</v>
+      </c>
+      <c r="C7" s="17">
+        <v>0.19853399999999999</v>
+      </c>
+      <c r="D7" s="17">
+        <v>0.57494000000000001</v>
+      </c>
+      <c r="E7" s="18">
+        <f t="shared" si="0"/>
+        <v>0.34531255435349772</v>
+      </c>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+    </row>
+    <row r="8" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B8" s="16">
+        <v>512</v>
+      </c>
+      <c r="C8" s="17">
+        <v>0.77720400000000001</v>
+      </c>
+      <c r="D8" s="17">
+        <v>0.576627</v>
+      </c>
+      <c r="E8" s="17">
+        <f>C8/D8</f>
+        <v>1.3478453142152553</v>
+      </c>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+    </row>
+    <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B9" s="16">
+        <f>B8*2</f>
+        <v>1024</v>
+      </c>
+      <c r="C9" s="17">
+        <v>3.1207699999999998</v>
+      </c>
+      <c r="D9" s="17">
+        <v>0.62615799999999999</v>
+      </c>
+      <c r="E9" s="17">
+        <f t="shared" ref="E9:E19" si="1">C9/D9</f>
+        <v>4.9839976491556444</v>
+      </c>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+    </row>
+    <row r="10" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B10" s="16">
+        <f t="shared" ref="B10:B19" si="2">B9*2</f>
+        <v>2048</v>
+      </c>
+      <c r="C10" s="17">
+        <v>12.122532</v>
+      </c>
+      <c r="D10" s="17">
+        <v>0.57819500000000001</v>
+      </c>
+      <c r="E10" s="19">
+        <f t="shared" si="1"/>
+        <v>20.966165394027964</v>
+      </c>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+    </row>
+    <row r="11" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B11" s="16">
+        <f t="shared" si="2"/>
+        <v>4096</v>
+      </c>
+      <c r="C11" s="17">
+        <v>49.986767</v>
+      </c>
+      <c r="D11" s="17">
+        <v>0.58285900000000002</v>
+      </c>
+      <c r="E11" s="19">
+        <f t="shared" si="1"/>
+        <v>85.761336789858262</v>
+      </c>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+    </row>
+    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B12" s="16">
+        <f t="shared" si="2"/>
+        <v>8192</v>
+      </c>
+      <c r="C12" s="17">
+        <v>202.46296000000001</v>
+      </c>
+      <c r="D12" s="17">
+        <v>0.65429499999999996</v>
+      </c>
+      <c r="E12" s="20">
+        <f t="shared" si="1"/>
+        <v>309.43681366967502</v>
+      </c>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+    </row>
+    <row r="13" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B13" s="16">
+        <f t="shared" si="2"/>
+        <v>16384</v>
+      </c>
+      <c r="C13" s="17">
+        <v>779.534896</v>
+      </c>
+      <c r="D13" s="17">
+        <v>0.66655299999999995</v>
+      </c>
+      <c r="E13" s="20">
+        <f t="shared" si="1"/>
+        <v>1169.5017440473603</v>
+      </c>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+    </row>
+    <row r="14" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B14" s="16">
+        <f t="shared" si="2"/>
+        <v>32768</v>
+      </c>
+      <c r="C14" s="17">
+        <v>3200.8664170000002</v>
+      </c>
+      <c r="D14" s="17">
+        <v>0.92805499999999996</v>
+      </c>
+      <c r="E14" s="20">
+        <f t="shared" si="1"/>
+        <v>3449.005088060514</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+    </row>
+    <row r="15" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B15" s="16">
+        <f t="shared" si="2"/>
+        <v>65536</v>
+      </c>
+      <c r="C15" s="21">
+        <f>4*3200</f>
+        <v>12800</v>
+      </c>
+      <c r="D15" s="17">
+        <v>1.5692269999999999</v>
+      </c>
+      <c r="E15" s="20">
+        <f t="shared" si="1"/>
+        <v>8156.882337609537</v>
+      </c>
+      <c r="F15" s="16"/>
+      <c r="G15" s="22"/>
+    </row>
+    <row r="16" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B16" s="16">
+        <f t="shared" si="2"/>
+        <v>131072</v>
+      </c>
+      <c r="C16" s="21">
+        <f>4*C15</f>
+        <v>51200</v>
+      </c>
+      <c r="D16" s="17">
+        <v>4.1981659999999996</v>
+      </c>
+      <c r="E16" s="20">
+        <f t="shared" si="1"/>
+        <v>12195.801690547731</v>
+      </c>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+    </row>
+    <row r="17" spans="2:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B17" s="16">
+        <f t="shared" si="2"/>
+        <v>262144</v>
+      </c>
+      <c r="C17" s="21">
+        <f>4*C16</f>
+        <v>204800</v>
+      </c>
+      <c r="D17" s="23">
+        <v>14.932665999999999</v>
+      </c>
+      <c r="E17" s="20">
+        <f t="shared" si="1"/>
+        <v>13714.89859881685</v>
+      </c>
+      <c r="F17" s="16"/>
+      <c r="G17" s="24"/>
+    </row>
+    <row r="18" spans="2:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B18" s="16">
+        <f t="shared" si="2"/>
+        <v>524288</v>
+      </c>
+      <c r="C18" s="21">
+        <f>4*C17</f>
+        <v>819200</v>
+      </c>
+      <c r="D18" s="23">
+        <v>56.032819000000003</v>
+      </c>
+      <c r="E18" s="20">
+        <f t="shared" si="1"/>
+        <v>14620.003323409446</v>
+      </c>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="19" spans="2:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B19" s="16">
+        <f t="shared" si="2"/>
+        <v>1048576</v>
+      </c>
+      <c r="C19" s="21">
+        <f>4*C18</f>
+        <v>3276800</v>
+      </c>
+      <c r="D19" s="23">
+        <v>222.23948999999999</v>
+      </c>
+      <c r="E19" s="20">
+        <f t="shared" si="1"/>
+        <v>14744.454282180004</v>
+      </c>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+    </row>
+    <row r="20" spans="2:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>